<commit_message>
cambios en las conexiones, lista en la pokedex de android
</commit_message>
<xml_diff>
--- a/Archivos/HorasDedicadas.xlsx
+++ b/Archivos/HorasDedicadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caoti\Documents\GitHub\TFG\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9144E523-2E05-4AE9-ABB9-0A849BFB39D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244F7C75-791A-4A2F-96B1-AB4CB9B0C3A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Minutos</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>Cambios menores al layout de la pokedex.</t>
+  </si>
+  <si>
+    <t>Crear listView de la pokedex y actividad intermedia.</t>
+  </si>
+  <si>
+    <t>Cambiar metodos de conexión para poder unirse en mitad de la partida y abandonar.</t>
+  </si>
+  <si>
+    <t>Cambiar conexiones para poder unirse y salirse en cualquier momento y evitar fallos.</t>
   </si>
 </sst>
 </file>
@@ -448,8 +457,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF896CE3-B8BD-43F6-BA2E-901BC648D50F}" name="Tabla1" displayName="Tabla1" ref="D4:F42" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="D4:F42" xr:uid="{B7C67675-289C-43E0-8C42-6E5BDE89F297}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF896CE3-B8BD-43F6-BA2E-901BC648D50F}" name="Tabla1" displayName="Tabla1" ref="D4:F45" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="D4:F45" xr:uid="{B7C67675-289C-43E0-8C42-6E5BDE89F297}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D5:F18">
     <sortCondition ref="D4:D18"/>
   </sortState>
@@ -725,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:J42"/>
+  <dimension ref="D3:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,11 +783,11 @@
       <c r="H5" s="10"/>
       <c r="I5" s="8">
         <f>SUM(Tabla1[Minutos])</f>
-        <v>1690</v>
+        <v>1900</v>
       </c>
       <c r="J5" s="7">
         <f>CONVERT(I5,"mn","hr")</f>
-        <v>28.166666666666668</v>
+        <v>31.666666666666668</v>
       </c>
     </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.25">
@@ -1186,6 +1195,39 @@
       </c>
       <c r="F42" s="1" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="6">
+        <v>44276</v>
+      </c>
+      <c r="E43" s="5">
+        <v>75</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D44" s="6">
+        <v>44276</v>
+      </c>
+      <c r="E44" s="5">
+        <v>40</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D45" s="6">
+        <v>44276</v>
+      </c>
+      <c r="E45" s="5">
+        <v>95</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hilo mensajes texto agregado a android
-Probar falta.
-Cambios menores en el XML..
</commit_message>
<xml_diff>
--- a/Archivos/HorasDedicadas.xlsx
+++ b/Archivos/HorasDedicadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caoti\Documents\GitHub\TFG\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244F7C75-791A-4A2F-96B1-AB4CB9B0C3A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D462B45-8382-4E6F-A207-4E176BF8687A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Minutos</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>Cambiar conexiones para poder unirse y salirse en cualquier momento y evitar fallos.</t>
+  </si>
+  <si>
+    <t>Primera reunión con César para hablar sobre el proyecto.</t>
+  </si>
+  <si>
+    <t>Agregar segundo hilo servidor al android para recibir cadenas de texto de lo sucedido en el turno.</t>
   </si>
 </sst>
 </file>
@@ -457,8 +463,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF896CE3-B8BD-43F6-BA2E-901BC648D50F}" name="Tabla1" displayName="Tabla1" ref="D4:F45" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="D4:F45" xr:uid="{B7C67675-289C-43E0-8C42-6E5BDE89F297}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF896CE3-B8BD-43F6-BA2E-901BC648D50F}" name="Tabla1" displayName="Tabla1" ref="D4:F47" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="D4:F47" xr:uid="{B7C67675-289C-43E0-8C42-6E5BDE89F297}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D5:F18">
     <sortCondition ref="D4:D18"/>
   </sortState>
@@ -734,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:J45"/>
+  <dimension ref="D3:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,11 +789,11 @@
       <c r="H5" s="10"/>
       <c r="I5" s="8">
         <f>SUM(Tabla1[Minutos])</f>
-        <v>1900</v>
+        <v>1980</v>
       </c>
       <c r="J5" s="7">
         <f>CONVERT(I5,"mn","hr")</f>
-        <v>31.666666666666668</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.25">
@@ -1228,6 +1234,28 @@
       </c>
       <c r="F45" s="1" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D46" s="6">
+        <v>44277</v>
+      </c>
+      <c r="E46" s="5">
+        <v>20</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D47" s="6">
+        <v>44277</v>
+      </c>
+      <c r="E47" s="5">
+        <v>60</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglado el hilo de mensajes
Falla a veces al morirse un pokemon (no es grave)
intentar mandar el end cuando pase
</commit_message>
<xml_diff>
--- a/Archivos/HorasDedicadas.xlsx
+++ b/Archivos/HorasDedicadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caoti\Documents\GitHub\TFG\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D462B45-8382-4E6F-A207-4E176BF8687A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08468ECF-FE5D-4DD3-BAD9-D3B2D9E4B3EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Minutos</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Agregar segundo hilo servidor al android para recibir cadenas de texto de lo sucedido en el turno.</t>
+  </si>
+  <si>
+    <t>Arreglar el hilo e investigar sobre el formato de texto.</t>
   </si>
 </sst>
 </file>
@@ -463,8 +466,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF896CE3-B8BD-43F6-BA2E-901BC648D50F}" name="Tabla1" displayName="Tabla1" ref="D4:F47" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="D4:F47" xr:uid="{B7C67675-289C-43E0-8C42-6E5BDE89F297}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF896CE3-B8BD-43F6-BA2E-901BC648D50F}" name="Tabla1" displayName="Tabla1" ref="D4:F48" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="D4:F48" xr:uid="{B7C67675-289C-43E0-8C42-6E5BDE89F297}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D5:F18">
     <sortCondition ref="D4:D18"/>
   </sortState>
@@ -740,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:J47"/>
+  <dimension ref="D3:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,11 +792,11 @@
       <c r="H5" s="10"/>
       <c r="I5" s="8">
         <f>SUM(Tabla1[Minutos])</f>
-        <v>1980</v>
+        <v>2070</v>
       </c>
       <c r="J5" s="7">
         <f>CONVERT(I5,"mn","hr")</f>
-        <v>33</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.25">
@@ -1256,6 +1259,17 @@
       </c>
       <c r="F47" s="1" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="6">
+        <v>44278</v>
+      </c>
+      <c r="E48" s="5">
+        <v>90</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
diagrama de clases agregado
</commit_message>
<xml_diff>
--- a/Archivos/HorasDedicadas.xlsx
+++ b/Archivos/HorasDedicadas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caoti\Documents\GitHub\TFG\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8F9E8B-BC29-4DC8-AEA9-E9A6CDFFEBCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732E6389-5AAE-4DB0-BCEF-FD55A687F008}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Minutos</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Redactar objetivos.</t>
+  </si>
+  <si>
+    <t>Redactar diagrama de clases memoria.</t>
   </si>
 </sst>
 </file>
@@ -487,8 +490,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF896CE3-B8BD-43F6-BA2E-901BC648D50F}" name="Tabla1" displayName="Tabla1" ref="D4:F55" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="D4:F55" xr:uid="{B7C67675-289C-43E0-8C42-6E5BDE89F297}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF896CE3-B8BD-43F6-BA2E-901BC648D50F}" name="Tabla1" displayName="Tabla1" ref="D4:F56" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="D4:F56" xr:uid="{B7C67675-289C-43E0-8C42-6E5BDE89F297}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D5:F18">
     <sortCondition ref="D4:D18"/>
   </sortState>
@@ -764,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:J55"/>
+  <dimension ref="D3:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,11 +816,11 @@
       <c r="H5" s="10"/>
       <c r="I5" s="8">
         <f>SUM(Tabla1[Minutos])</f>
-        <v>2495</v>
+        <v>2615</v>
       </c>
       <c r="J5" s="7">
         <f>CONVERT(I5,"mn","hr")</f>
-        <v>41.583333333333336</v>
+        <v>43.583333333333336</v>
       </c>
     </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.25">
@@ -1368,6 +1371,17 @@
       </c>
       <c r="F55" s="1" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D56" s="6">
+        <v>44307</v>
+      </c>
+      <c r="E56" s="5">
+        <v>120</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>